<commit_message>
classificador e verificacao de acertos
</commit_message>
<xml_diff>
--- a/base_acai.xlsx
+++ b/base_acai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellenbeatriz/Desktop/INSPER/2º Semestre/Projeto-2_CD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F01EF06A-7606-9B46-844E-5B199D4795D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72276BD-0282-4744-B844-25CA7266CEFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="753">
   <si>
     <t>um açaí de um litro agora cairia muito bem😋😋😋</t>
   </si>
@@ -2378,6 +2378,9 @@
   </si>
   <si>
     <t>nao gosto de acai</t>
+  </si>
+  <si>
+    <t>Teste</t>
   </si>
 </sst>
 </file>
@@ -2783,7 +2786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B451"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+    <sheetView zoomScale="99" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -6412,9 +6415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1E1A82E-BE7A-CD46-A18F-B48FE72093C4}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6423,7 +6424,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>745</v>
+        <v>752</v>
       </c>
       <c r="B1" t="s">
         <v>746</v>

</xml_diff>